<commit_message>
[Add] Renpy branch save 25.06.11
</commit_message>
<xml_diff>
--- a/My project (2)/Assets/Data/Data.xlsx
+++ b/My project (2)/Assets/Data/Data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Project\ProjectBS\ProjectBS\Assets\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\Unity_Git\UnityBasic2\My project (2)\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5624E0-82EA-45F1-8ED0-E4766F84D709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703DDE43-9D04-4DE2-A665-9209923B85BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="210" windowWidth="20910" windowHeight="15105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="3" r:id="rId1"/>
+    <sheet name="Dialogue" sheetId="1" r:id="rId2"/>
+    <sheet name="Character" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,17 +27,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Name_S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID_I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bbno</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dialogue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슈로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카즈사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Img/Shuro_00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Img/Kazusa_00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discription</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화조풍월부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방과후 디저트부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슈로_기본표정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카즈사_기본표정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Img/Shuro_01</t>
+  </si>
+  <si>
+    <t>Img/Shuro_02</t>
+  </si>
+  <si>
+    <t>슈로_웃는표정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슈로_궁금한표정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BG_CraftChamber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Img/Kazusa_01</t>
+  </si>
+  <si>
+    <t>카즈사_웃는표정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Img/Kazusa_02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카즈사_궁금한표정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지원님 준모님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지/원님 준/모님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지/원/님 준/모/님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지원/님/준모/님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지==============원==============준=============모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -79,8 +190,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -360,33 +477,282 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1CEAA6-3302-4E8D-BD86-5BCD14C94795}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.75" style="1" customWidth="1"/>
+    <col min="2" max="4" width="24.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="104" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10201</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10102</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10103</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10101</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10202</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24494642-9FC4-4D0C-B88A-71C71EAA3505}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="30.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>10101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>10102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>10103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>10201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>10202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>10203</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>